<commit_message>
Added visual representations, report and circuits.
</commit_message>
<xml_diff>
--- a/NRSData.xlsx
+++ b/NRSData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +95,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -105,196 +110,376 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Combination of Pre-emphasis and De-emphasis filter </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet2!$B$3:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000.0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4000.0</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5000.0</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6000.0</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8000.0</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>150.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1500.0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1300.0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1800.0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2500.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>120.0</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$26</c:f>
+              <c:f>Sheet2!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.57436122400334599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.3200778789128869E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>100, -0.574</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6689352525461555E-2"/>
+                  <c:y val="0.15316639752509326"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>10000, -0.825</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-0.574361224003346</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.106229081576819</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.223745299464145</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.197583777458633</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$3:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-0.57436122400334599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21278233473259719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10622908157681896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.22374529946414465</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.1975837774586331</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>-2.137304721431442</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>-3.195283691450395</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-3.841239939551761</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.840004481241157</c:v>
+                  <c:v>-3.1952836914503955</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-3.279121172114239</c:v>
+                  <c:v>-3.8412399395517611</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.979983339794976</c:v>
+                  <c:v>-3.8400044812411567</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.482881059592127</c:v>
+                  <c:v>-3.2791211721142388</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.572827453012822</c:v>
+                  <c:v>-1.9799833397949755</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.534871894403971</c:v>
+                  <c:v>-1.1975837774586331</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.434124355728497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.739951328907113</c:v>
+                  <c:v>1.4351036085696367</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.77589410218033</c:v>
+                  <c:v>2.4828810595921271</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.735123369008234</c:v>
+                  <c:v>3.4430897544482466</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.545670048096831</c:v>
+                  <c:v>4.572827453012823</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.824966106848655</c:v>
+                  <c:v>4.5348718944039712</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.212782334732597</c:v>
+                  <c:v>4.4341243557284971</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0</c:v>
+                  <c:v>3.7399513289071136</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-1.197583777458633</c:v>
+                  <c:v>2.7758941021803301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.435103608569637</c:v>
+                  <c:v>1.7351233690082344</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.443089754448247</c:v>
+                  <c:v>0.54567004809683084</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.82496610684865535</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -304,55 +489,106 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2035079640"/>
-        <c:axId val="-2034971624"/>
+        <c:axId val="76980608"/>
+        <c:axId val="76982912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2035079640"/>
+        <c:axId val="76980608"/>
         <c:scaling>
-          <c:logBase val="10.0"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="100.0"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2034971624"/>
+        <c:crossAx val="76982912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2034971624"/>
+        <c:axId val="76982912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>20log│H(j</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ω)│ (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>dB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2035079640"/>
+        <c:crossAx val="76980608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -362,16 +598,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -715,513 +951,508 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="B2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F3" activeCellId="2" sqref="B3:B27 F3 F3:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:6">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2">
+    <row r="3" spans="2:6">
+      <c r="B3" s="2">
         <v>100</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C3" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D3" s="2">
         <v>1.141</v>
       </c>
-      <c r="D2" s="2">
-        <f>C2/B2</f>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E27" si="0">D3/C3</f>
         <v>0.93601312551271532</v>
       </c>
-      <c r="E2" s="2">
-        <f>20*LOG(D2)</f>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F27" si="1">20*LOG(E3)</f>
         <v>-0.57436122400334599</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
+    <row r="4" spans="2:6">
+      <c r="B4" s="1">
+        <v>120</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="1">
+        <v>150</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0247999999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21278233473259719</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="2">
         <v>200</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C6" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D6" s="2">
         <v>1.234</v>
       </c>
-      <c r="D3" s="2">
-        <f t="shared" ref="D3:D26" si="0">C3/B3</f>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
         <v>1.0123051681706317</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E26" si="1">20*LOG(D3)</f>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
         <v>0.10622908157681896</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
+    <row r="7" spans="2:6">
+      <c r="B7" s="2">
         <v>300</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C7" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D7" s="2">
         <v>1.1879999999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>0.97456931911402778</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>-0.22374529946414465</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2">
+    <row r="8" spans="2:6">
+      <c r="B8" s="2">
         <v>400</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C8" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D8" s="2">
         <v>1.0620000000000001</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.87120590648072194</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>-1.1975837774586331</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
+    <row r="9" spans="2:6">
+      <c r="B9" s="1">
         <v>500</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C9" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D9" s="2">
         <v>0.95309999999999995</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.78187038556193589</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>-2.137304721431442</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
+    <row r="10" spans="2:6">
+      <c r="B10" s="1">
         <v>600</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C10" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D10" s="2">
         <v>0.84379999999999999</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>0.69220672682526652</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>-3.1952836914503955</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
+    <row r="11" spans="2:6">
+      <c r="B11" s="1">
         <v>700</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C11" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D11" s="2">
         <v>0.70299999999999996</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>0.64259597806215718</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>-3.8412399395517611</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2">
+    <row r="12" spans="2:6">
+      <c r="B12" s="2">
         <v>800</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C12" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D12" s="2">
         <v>0.70309999999999995</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>0.64268738574040207</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>-3.8400044812411567</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
+    <row r="13" spans="2:6">
+      <c r="B13" s="1">
         <v>900</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C13" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D13" s="2">
         <v>0.75</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>0.68555758683729429</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>-3.2791211721142388</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
+    <row r="14" spans="2:6">
+      <c r="B14" s="1">
         <v>1000</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C14" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D14" s="2">
         <v>0.871</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>0.79616087751371112</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>-1.9799833397949755</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1">
+    <row r="15" spans="2:6">
+      <c r="B15" s="1">
+        <v>1300</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.87120590648072194</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.1975837774586331</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="1">
+        <v>1800</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.4379999999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1796554552912222</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4351036085696367</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="1">
         <v>2000</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C18" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D18" s="2">
         <v>1.456</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>1.3308957952468006</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>2.4828810595921271</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1">
+    <row r="19" spans="2:6">
+      <c r="B19" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.8120000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4864643150123051</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4430897544482466</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="1">
         <v>3000</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C20" s="2">
         <v>0.60899999999999999</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D20" s="2">
         <v>1.0309999999999999</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>1.6929392446633824</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>4.572827453012823</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1">
+    <row r="21" spans="2:6">
+      <c r="B21" s="1">
         <v>4000</v>
       </c>
-      <c r="B14" s="2">
+      <c r="C21" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D21" s="2">
         <v>1.8440000000000001</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>1.6855575868372943</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F21" s="2">
         <f t="shared" si="1"/>
         <v>4.5348718944039712</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1">
+    <row r="22" spans="2:6">
+      <c r="B22" s="1">
         <v>5000</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1.2190000000000001</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2.0310000000000001</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6661197703035275</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="1"/>
-        <v>4.4341243557284971</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1">
-        <v>6000</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1.2190000000000001</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1.875</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5381460213289579</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="1"/>
-        <v>3.7399513289071136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1">
-        <v>7000</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1.2030000000000001</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1.6559999999999999</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3765586034912716</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>2.7758941021803301</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1">
-        <v>8000</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1.2030000000000001</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1.4690000000000001</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2211138819617622</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7351233690082344</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1">
-        <v>9000</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1.2030000000000001</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1.2809999999999999</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0648379052369077</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54567004809683084</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1">
-        <v>10000</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1.2030000000000001</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1.0940000000000001</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.90939318370739819</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.82496610684865535</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1">
-        <v>150</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1.2809999999999999</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0247999999999999</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21278233473259719</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1">
-        <v>1500</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1.2190000000000001</v>
       </c>
       <c r="C22" s="2">
         <v>1.2190000000000001</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.0310000000000001</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1">
-        <v>1300</v>
-      </c>
-      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6661197703035275</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4341243557284971</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C23" s="2">
         <v>1.2190000000000001</v>
       </c>
-      <c r="C23" s="2">
-        <v>1.0620000000000001</v>
-      </c>
       <c r="D23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.87120590648072194</v>
+        <v>1.875</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="1"/>
-        <v>-1.1975837774586331</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1">
-        <v>1800</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1.2190000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.5381460213289579</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="1"/>
+        <v>3.7399513289071136</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="1">
+        <v>7000</v>
       </c>
       <c r="C24" s="2">
-        <v>1.4379999999999999</v>
+        <v>1.2030000000000001</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1796554552912222</v>
+        <v>1.6559999999999999</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4351036085696367</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1">
-        <v>2500</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1.2190000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.3765586034912716</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7758941021803301</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="1">
+        <v>8000</v>
       </c>
       <c r="C25" s="2">
-        <v>1.8120000000000001</v>
+        <v>1.2030000000000001</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>1.4864643150123051</v>
+        <v>1.4690000000000001</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="1"/>
-        <v>3.4430897544482466</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1">
-        <v>120</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1.25</v>
+        <f t="shared" si="0"/>
+        <v>1.2211138819617622</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7351233690082344</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="1">
+        <v>9000</v>
       </c>
       <c r="C26" s="2">
-        <v>1.25</v>
+        <v>1.2030000000000001</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.2809999999999999</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.0648379052369077</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.54567004809683084</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.2030000000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.90939318370739819</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.82496610684865535</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>